<commit_message>
Updated BOM Part 1
</commit_message>
<xml_diff>
--- a/Hardware/Mood-Light-Perhaps-BOM.xlsx
+++ b/Hardware/Mood-Light-Perhaps-BOM.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/Git/Tasks-Tutorials-Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadrezqalla/Desktop/Arduino Pro/Mood-Light-Perhaps/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F0319-899B-F545-ABC0-B856698FB7B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A755D0-616A-8247-93A0-E1751C36D6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -429,7 +440,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>BOM #</t>
   </si>
@@ -603,17 +614,148 @@
   </si>
   <si>
     <t>Design Name -- Revision Code / Designer or Organization Name</t>
+  </si>
+  <si>
+    <t>ATmega328</t>
+  </si>
+  <si>
+    <t>AVR AVR® ATmega Microcontroller IC 8-Bit 20MHz 32KB (16K x 16) FLASH 32-TQFP (7x7)</t>
+  </si>
+  <si>
+    <t>32-TQFP (7x7)</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AUR</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AURCT-ND</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>100k Resistor</t>
+  </si>
+  <si>
+    <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100KCT-ND</t>
+  </si>
+  <si>
+    <t>2k Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603FT200K</t>
+  </si>
+  <si>
+    <t>RMCF0603FT200KTR-ND</t>
+  </si>
+  <si>
+    <t>205 Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603FT205R</t>
+  </si>
+  <si>
+    <t>738-RMCF0603FT205RTR-ND</t>
+  </si>
+  <si>
+    <t>2 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>205 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>2.2u capacitor</t>
+  </si>
+  <si>
+    <t>2.2µF ±10% 16V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>CL10A225KO8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1040-1-ND</t>
+  </si>
+  <si>
+    <t>4.7 uF Capacitor</t>
+  </si>
+  <si>
+    <t>red 622nm LED Indication - Discrete 2.2V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>CL10A475KO8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1784-1-ND</t>
+  </si>
+  <si>
+    <t>0.1µF ±5% 16V Ceramic Capacitor X7R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R7BB104</t>
+  </si>
+  <si>
+    <t>311-1776-1-ND</t>
+  </si>
+  <si>
+    <t>0.1 uF Capacitor</t>
+  </si>
+  <si>
+    <t>22pF Capacitor</t>
+  </si>
+  <si>
+    <t>22 pF ±5% 50V Ceramic Capacitor C0G, NP0 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
+    <t>478-1167-2-ND</t>
+  </si>
+  <si>
+    <t>06035A220JAT2A</t>
+  </si>
+  <si>
+    <t>Red 8x8 LED Matrix</t>
+  </si>
+  <si>
+    <t>Small 1.2" 8x8 Ultra Bright Red LED Matrix - KWM-30881CVB</t>
+  </si>
+  <si>
+    <t>16-Pin THT</t>
+  </si>
+  <si>
+    <t>Luckylight</t>
+  </si>
+  <si>
+    <t>KWM-30881CVB</t>
+  </si>
+  <si>
+    <t>Adafruit Industries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -686,6 +828,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,7 +1011,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -894,6 +1049,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1314,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1325,13 +1485,13 @@
     <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
@@ -1355,14 +1515,14 @@
         <v>14</v>
       </c>
       <c r="M1" s="6">
-        <f>SUM(M3:M77)</f>
-        <v>2.48</v>
+        <f>SUM(M3:M76)</f>
+        <v>10.54</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="O1" s="6">
-        <f>SUM(O3:O77)</f>
+        <f>SUM(O3:O76)</f>
         <v>1.1271</v>
       </c>
     </row>
@@ -1706,10 +1866,421 @@
         <v>1.8499999999999999E-2</v>
       </c>
     </row>
+    <row r="10" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="16">
+        <v>2.14</v>
+      </c>
+      <c r="L10" s="15">
+        <v>1</v>
+      </c>
+      <c r="M10" s="16">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="15">
+        <v>603</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>4</v>
+      </c>
+      <c r="M11" s="16">
+        <f>K11*L11</f>
+        <v>0.4</v>
+      </c>
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="15">
+        <v>603</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="16">
+        <f>L12*K12</f>
+        <v>0.1</v>
+      </c>
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="15">
+        <v>603</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="17">
+        <f>L13*K13</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="15">
+        <v>603</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>8</v>
+      </c>
+      <c r="M14" s="17">
+        <f>L14*K14</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="15">
+        <v>603</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16">
+        <f>K15*L15</f>
+        <v>0.2</v>
+      </c>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" ht="12" x14ac:dyDescent="0.15">
+      <c r="B16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="15">
+        <v>603</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="L16" s="18">
+        <v>1</v>
+      </c>
+      <c r="M16" s="16">
+        <f t="shared" ref="M16:M17" si="2">K16*L16</f>
+        <v>0.03</v>
+      </c>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="2:14" ht="12" x14ac:dyDescent="0.15">
+      <c r="B17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="15">
+        <v>603</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2</v>
+      </c>
+      <c r="M17" s="16">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="2:14" ht="12" x14ac:dyDescent="0.15">
+      <c r="B18" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="15">
+        <v>603</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
+      <c r="M18" s="16">
+        <f>L18*K18</f>
+        <v>0.06</v>
+      </c>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1">
+        <v>603</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2</v>
+      </c>
+      <c r="M19" s="19">
+        <f>L19*K19</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="12" x14ac:dyDescent="0.15">
+      <c r="B20" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="15">
+        <v>455</v>
+      </c>
+      <c r="K20" s="16">
+        <v>3.95</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="16">
+        <f>L20*K20</f>
+        <v>3.95</v>
+      </c>
+      <c r="N20" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>